<commit_message>
Modificaciones minimas a la interfaz de usuario e interfaz final
</commit_message>
<xml_diff>
--- a/src/data/DatosExcel.xlsx
+++ b/src/data/DatosExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianvicente/Desktop/La Salle Oaxaca/5º_Semestre/Programacion para plataforma web/Parcial 3/appMeteorologica/src/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianvicente/Desktop/La Salle Oaxaca/5º_Semestre/Ingenieria en software 2/Parcial 3/appMeteorologica/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38D79E5F-9400-2646-999C-DD7CAC182787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC40703-EE3B-EA40-A52C-3E148034EC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{202E6D57-5EF8-3944-8A45-FC472739CD61}"/>
+    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{DAD5800F-4358-D948-84C1-8A39ECFAFBD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,27 +36,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>lunes</t>
+    <t>Lunes</t>
   </si>
   <si>
-    <t>martes</t>
+    <t>Martes</t>
   </si>
   <si>
-    <t>miercoles</t>
+    <t>Miercoles</t>
   </si>
   <si>
-    <t>jueves</t>
+    <t>Jueves</t>
   </si>
   <si>
-    <t>viernes</t>
-  </si>
-  <si>
-    <t>sabado</t>
-  </si>
-  <si>
-    <t>domingo</t>
+    <t>Viernes</t>
   </si>
 </sst>
 </file>
@@ -407,11 +401,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42339AB8-BD9E-064D-A863-65410D90A4BC}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCABC40-10A3-6049-9FF6-C6FCA896E632}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -421,7 +415,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>26.7</v>
+        <v>26.2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -429,7 +423,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>25.8</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -437,7 +431,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>23.9</v>
+        <v>20.6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -445,7 +439,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>25.7</v>
+        <v>23.4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -453,23 +447,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>19.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>25.1</v>
+        <v>19.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>